<commit_message>
Update VERA - Referentiedata - 2021-11-05.xlsx
Relatierolsoorten aangevuld n.a.v. RFC SK038
</commit_message>
<xml_diff>
--- a/Referentiedata/VERA - Referentiedata - 2021-11-05.xlsx
+++ b/Referentiedata/VERA - Referentiedata - 2021-11-05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martijn\AppData\Local\GitHubDesktop\app-2.9.0\VERA\VERA-Standaard\Referentiedata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3130B7F6-A9C4-4F85-9191-296241F4AEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CF9C97-B4DA-48ED-8645-5C8A4C9A042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7002" uniqueCount="3767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7022" uniqueCount="3777">
   <si>
     <t>Referentiedatasoort</t>
   </si>
@@ -11390,6 +11390,36 @@
   </si>
   <si>
     <t>Projectbudgetregel is een optelling van één of meer onderliggende kosten- of opbrengstenregels binnen de stichtingskosten hiërarchie</t>
+  </si>
+  <si>
+    <t>ASS</t>
+  </si>
+  <si>
+    <t>Woonconsulent</t>
+  </si>
+  <si>
+    <t>De woonconsulent voor het betreffende vastgoed</t>
+  </si>
+  <si>
+    <t>HME</t>
+  </si>
+  <si>
+    <t>Huismeester</t>
+  </si>
+  <si>
+    <t>De huismeester voor het betreffende vastgoed</t>
+  </si>
+  <si>
+    <t>Opzichter</t>
+  </si>
+  <si>
+    <t>De opzichter voor het betreffende vastgoed</t>
+  </si>
+  <si>
+    <t>Assetmanager</t>
+  </si>
+  <si>
+    <t>De assetmanager voor het betreffende vastgoed</t>
   </si>
 </sst>
 </file>
@@ -11547,7 +11577,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -11698,6 +11728,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -12094,8 +12125,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1061" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:K1061" xr:uid="{8B075628-E833-48DC-8779-68AB54AC5BC1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1065" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:K1065" xr:uid="{8B075628-E833-48DC-8779-68AB54AC5BC1}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{845F9FC6-EA7E-42C8-9954-6B75834B5282}" name="Referentiedatasoort" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{ABFA2115-257A-4C72-8D5D-B12F03C0BC13}" name="Sortering" dataDxfId="18"/>
@@ -12467,10 +12498,10 @@
   <sheetPr codeName="Blad1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L1061"/>
+  <dimension ref="A1:L1065"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A840" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1038" sqref="A1038"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34668,6 +34699,98 @@
       </c>
       <c r="J1061" s="10"/>
       <c r="K1061" s="10"/>
+    </row>
+    <row r="1062" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1062" s="36" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B1062" s="10"/>
+      <c r="C1062" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1062" s="11" t="s">
+        <v>3768</v>
+      </c>
+      <c r="E1062" s="54" t="s">
+        <v>3769</v>
+      </c>
+      <c r="F1062" s="11"/>
+      <c r="G1062" s="11"/>
+      <c r="H1062" s="10"/>
+      <c r="I1062" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1062" s="10"/>
+      <c r="K1062" s="10"/>
+    </row>
+    <row r="1063" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1063" s="36" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B1063" s="10"/>
+      <c r="C1063" s="10" t="s">
+        <v>3770</v>
+      </c>
+      <c r="D1063" s="11" t="s">
+        <v>3771</v>
+      </c>
+      <c r="E1063" s="54" t="s">
+        <v>3772</v>
+      </c>
+      <c r="F1063" s="11"/>
+      <c r="G1063" s="11"/>
+      <c r="H1063" s="10"/>
+      <c r="I1063" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1063" s="10"/>
+      <c r="K1063" s="10"/>
+    </row>
+    <row r="1064" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1064" s="36" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B1064" s="10"/>
+      <c r="C1064" s="10" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D1064" s="11" t="s">
+        <v>3773</v>
+      </c>
+      <c r="E1064" s="54" t="s">
+        <v>3774</v>
+      </c>
+      <c r="F1064" s="11"/>
+      <c r="G1064" s="11"/>
+      <c r="H1064" s="10"/>
+      <c r="I1064" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1064" s="10"/>
+      <c r="K1064" s="10"/>
+    </row>
+    <row r="1065" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1065" s="36" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B1065" s="10"/>
+      <c r="C1065" s="10" t="s">
+        <v>3767</v>
+      </c>
+      <c r="D1065" s="11" t="s">
+        <v>3775</v>
+      </c>
+      <c r="E1065" s="54" t="s">
+        <v>3776</v>
+      </c>
+      <c r="F1065" s="11"/>
+      <c r="G1065" s="11"/>
+      <c r="H1065" s="10"/>
+      <c r="I1065" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1065" s="10"/>
+      <c r="K1065" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -40912,21 +41035,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFD438D9B9ABE14A977C2E01E1E997E9" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="238b4f00df057bc2742cc7aff66473ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="41b44f4d-acd5-45c0-8ca7-9032ca64d707" xmlns:ns3="bc2bfcf0-0204-42b7-916d-bc08fc5e6372" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfb8db5c6f5549a83cd0326992bdc891" ns2:_="" ns3:_="">
     <xsd:import namespace="41b44f4d-acd5-45c0-8ca7-9032ca64d707"/>
@@ -41129,24 +41237,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9FCA9DB-B654-4D97-A1BC-1B4528FD4E25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41163,4 +41269,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>